<commit_message>
`Refactored insert_data_to_db function to remove duplicate checks and row-by-row inserts, and added batch execution with retry mechanism.`
</commit_message>
<xml_diff>
--- a/static/demo excel/Demo_Excel.xlsx
+++ b/static/demo excel/Demo_Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soham3.Patil\Desktop\PrintDesk\static\demo excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreyas1.Sawant\Desktop\PrintDesk\static\demo excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D9DBBFF-E057-4690-950D-FF46308BD9CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892A0724-FCA4-4747-B979-7C6CBA72AC7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{FCB9B742-7704-466D-AC72-AA101E9C75A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">User Name </t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>01-04-2025 00:34:01</t>
-  </si>
-  <si>
-    <t>01-04-2025 00:37:27</t>
   </si>
   <si>
     <t>User1</t>
@@ -128,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -137,6 +131,9 @@
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -467,7 +464,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,38 +493,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="E2" s="4">
+        <v>46026.023622685185</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>50000</v>
+      </c>
+      <c r="E3" s="4">
+        <v>46026.026006944441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Refactored data processing and upload functionality in routes.py and data_processing.py, updated date parsing and duplicate row removal logic, and added logging and error handling.`
</commit_message>
<xml_diff>
--- a/static/demo excel/Demo_Excel.xlsx
+++ b/static/demo excel/Demo_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shreyas1.Sawant\Desktop\PrintDesk\static\demo excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892A0724-FCA4-4747-B979-7C6CBA72AC7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD45979C-AB99-4DCF-8C4C-611FD6A0ED64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{FCB9B742-7704-466D-AC72-AA101E9C75A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">User Name </t>
   </si>
@@ -58,13 +58,22 @@
   </si>
   <si>
     <t>Host2</t>
+  </si>
+  <si>
+    <t>13-06-2024 11:13:45</t>
+  </si>
+  <si>
+    <t>13-06-2024 11:13:23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +95,11 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -118,11 +132,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -133,8 +160,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AA05FC-230C-417D-BE38-2AB2C96B43EC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,10 +507,10 @@
     <col min="2" max="2" width="21.7265625" customWidth="1"/>
     <col min="3" max="3" width="26.453125" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,11 +523,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -506,11 +540,12 @@
       <c r="D2" s="3">
         <v>1000</v>
       </c>
-      <c r="E2" s="4">
-        <v>46026.023622685185</v>
-      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -523,9 +558,14 @@
       <c r="D3" s="3">
         <v>50000</v>
       </c>
-      <c r="E3" s="4">
-        <v>46026.026006944441</v>
-      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E3">
@@ -534,5 +574,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>